<commit_message>
Fix Dailyreport page: save file scan, key code check
</commit_message>
<xml_diff>
--- a/py/direction_sheet.xlsx
+++ b/py/direction_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\diereport\ex0.11\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8766328A-6AEC-47E1-9841-054CC28BEE73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8885CBE7-90A9-4071-B01B-D1C379416122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="12420" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="print" sheetId="1" r:id="rId1"/>
@@ -2564,10 +2564,439 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="79" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2590,435 +3019,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="79" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3439,8 +3439,8 @@
   </sheetPr>
   <dimension ref="B1:AI162"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="40" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="20.25"/>
@@ -3469,28 +3469,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="66.75" customHeight="1" thickBot="1">
-      <c r="B1" s="266" t="s">
+      <c r="B1" s="370" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="267"/>
-      <c r="D1" s="267"/>
-      <c r="E1" s="267"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="268"/>
-      <c r="N1" s="268"/>
-      <c r="O1" s="267"/>
-      <c r="P1" s="267"/>
-      <c r="Q1" s="267"/>
-      <c r="R1" s="267"/>
-      <c r="S1" s="267"/>
-      <c r="T1" s="267"/>
-      <c r="U1" s="269"/>
+      <c r="C1" s="371"/>
+      <c r="D1" s="371"/>
+      <c r="E1" s="371"/>
+      <c r="F1" s="372"/>
+      <c r="G1" s="372"/>
+      <c r="H1" s="372"/>
+      <c r="I1" s="372"/>
+      <c r="J1" s="372"/>
+      <c r="K1" s="372"/>
+      <c r="L1" s="372"/>
+      <c r="M1" s="372"/>
+      <c r="N1" s="372"/>
+      <c r="O1" s="371"/>
+      <c r="P1" s="371"/>
+      <c r="Q1" s="371"/>
+      <c r="R1" s="371"/>
+      <c r="S1" s="371"/>
+      <c r="T1" s="371"/>
+      <c r="U1" s="373"/>
     </row>
     <row r="2" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
       <c r="B2" s="252" t="s">
@@ -3507,26 +3507,26 @@
         <f>input!D8</f>
         <v>0</v>
       </c>
-      <c r="F2" s="270"/>
-      <c r="G2" s="271"/>
+      <c r="F2" s="374"/>
+      <c r="G2" s="375"/>
       <c r="H2" s="240"/>
       <c r="I2" s="139"/>
       <c r="J2" s="240"/>
       <c r="K2" s="140"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="289"/>
+      <c r="L2" s="375"/>
+      <c r="M2" s="320"/>
       <c r="N2" s="141"/>
-      <c r="O2" s="346" t="s">
+      <c r="O2" s="287" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="347"/>
-      <c r="Q2" s="346" t="s">
+      <c r="P2" s="323"/>
+      <c r="Q2" s="287" t="s">
         <v>125</v>
       </c>
-      <c r="R2" s="350"/>
-      <c r="S2" s="350"/>
-      <c r="T2" s="350"/>
-      <c r="U2" s="347"/>
+      <c r="R2" s="325"/>
+      <c r="S2" s="325"/>
+      <c r="T2" s="325"/>
+      <c r="U2" s="323"/>
     </row>
     <row r="3" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
       <c r="B3" s="236" t="s">
@@ -3543,24 +3543,24 @@
         <f>input!D9</f>
         <v>0</v>
       </c>
-      <c r="F3" s="270"/>
-      <c r="G3" s="271"/>
+      <c r="F3" s="374"/>
+      <c r="G3" s="375"/>
       <c r="H3" s="240"/>
       <c r="I3" s="140"/>
       <c r="J3" s="240"/>
       <c r="K3" s="44"/>
-      <c r="L3" s="271"/>
-      <c r="M3" s="289"/>
+      <c r="L3" s="375"/>
+      <c r="M3" s="320"/>
       <c r="N3" s="141"/>
-      <c r="O3" s="348" t="s">
+      <c r="O3" s="289" t="s">
         <v>131</v>
       </c>
-      <c r="P3" s="349"/>
-      <c r="Q3" s="348"/>
-      <c r="R3" s="351"/>
-      <c r="S3" s="351"/>
-      <c r="T3" s="351"/>
-      <c r="U3" s="349"/>
+      <c r="P3" s="324"/>
+      <c r="Q3" s="289"/>
+      <c r="R3" s="326"/>
+      <c r="S3" s="326"/>
+      <c r="T3" s="326"/>
+      <c r="U3" s="324"/>
     </row>
     <row r="4" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
       <c r="B4" s="25"/>
@@ -3568,17 +3568,17 @@
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
       <c r="F4" s="210"/>
-      <c r="G4" s="304" t="s">
+      <c r="G4" s="403" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="305"/>
-      <c r="I4" s="305"/>
-      <c r="J4" s="306"/>
-      <c r="K4" s="304" t="s">
+      <c r="H4" s="404"/>
+      <c r="I4" s="404"/>
+      <c r="J4" s="405"/>
+      <c r="K4" s="403" t="s">
         <v>142</v>
       </c>
-      <c r="L4" s="305"/>
-      <c r="M4" s="306"/>
+      <c r="L4" s="404"/>
+      <c r="M4" s="405"/>
       <c r="N4" s="143"/>
       <c r="O4" s="200" t="s">
         <v>83</v>
@@ -3586,24 +3586,24 @@
       <c r="P4" s="201" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="346" t="s">
+      <c r="Q4" s="287" t="s">
         <v>126</v>
       </c>
-      <c r="R4" s="350"/>
-      <c r="S4" s="350"/>
-      <c r="T4" s="350"/>
-      <c r="U4" s="347"/>
+      <c r="R4" s="325"/>
+      <c r="S4" s="325"/>
+      <c r="T4" s="325"/>
+      <c r="U4" s="323"/>
     </row>
     <row r="5" spans="2:31" ht="28.5" customHeight="1">
-      <c r="B5" s="290" t="s">
+      <c r="B5" s="303" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="292">
+      <c r="C5" s="391">
         <f>input!D6</f>
         <v>0</v>
       </c>
-      <c r="D5" s="293"/>
-      <c r="E5" s="294"/>
+      <c r="D5" s="392"/>
+      <c r="E5" s="393"/>
       <c r="F5" s="135"/>
       <c r="G5" s="145" t="s">
         <v>2</v>
@@ -3624,23 +3624,23 @@
       <c r="L5" s="193" t="s">
         <v>102</v>
       </c>
-      <c r="M5" s="318" t="s">
+      <c r="M5" s="345" t="s">
         <v>133</v>
       </c>
       <c r="N5" s="135"/>
-      <c r="O5" s="314"/>
-      <c r="P5" s="316"/>
-      <c r="Q5" s="322"/>
-      <c r="R5" s="323"/>
-      <c r="S5" s="323"/>
-      <c r="T5" s="323"/>
-      <c r="U5" s="324"/>
+      <c r="O5" s="341"/>
+      <c r="P5" s="343"/>
+      <c r="Q5" s="351"/>
+      <c r="R5" s="352"/>
+      <c r="S5" s="352"/>
+      <c r="T5" s="352"/>
+      <c r="U5" s="353"/>
     </row>
     <row r="6" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
-      <c r="B6" s="291"/>
-      <c r="C6" s="295"/>
-      <c r="D6" s="296"/>
-      <c r="E6" s="297"/>
+      <c r="B6" s="304"/>
+      <c r="C6" s="394"/>
+      <c r="D6" s="395"/>
+      <c r="E6" s="396"/>
       <c r="F6" s="135"/>
       <c r="G6" s="187">
         <v>6061</v>
@@ -3658,30 +3658,30 @@
         <f>input!D13</f>
         <v>0</v>
       </c>
-      <c r="L6" s="412">
+      <c r="L6" s="257">
         <f>ROUND(input!D14,2)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="319"/>
+      <c r="M6" s="346"/>
       <c r="N6" s="137"/>
-      <c r="O6" s="315"/>
-      <c r="P6" s="317"/>
-      <c r="Q6" s="325"/>
-      <c r="R6" s="326"/>
-      <c r="S6" s="326"/>
-      <c r="T6" s="326"/>
-      <c r="U6" s="327"/>
+      <c r="O6" s="342"/>
+      <c r="P6" s="344"/>
+      <c r="Q6" s="354"/>
+      <c r="R6" s="355"/>
+      <c r="S6" s="355"/>
+      <c r="T6" s="355"/>
+      <c r="U6" s="356"/>
     </row>
     <row r="7" spans="2:31" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B7" s="287" t="s">
+      <c r="B7" s="305" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="298">
+      <c r="C7" s="397">
         <f>input!D7</f>
         <v>0</v>
       </c>
-      <c r="D7" s="299"/>
-      <c r="E7" s="300"/>
+      <c r="D7" s="398"/>
+      <c r="E7" s="399"/>
       <c r="F7" s="135"/>
       <c r="G7" s="187">
         <v>6063</v>
@@ -3702,30 +3702,30 @@
       <c r="L7" s="197" t="s">
         <v>104</v>
       </c>
-      <c r="M7" s="320">
+      <c r="M7" s="347">
         <f>input!D11</f>
         <v>0</v>
       </c>
       <c r="N7" s="138"/>
-      <c r="O7" s="337" t="s">
+      <c r="O7" s="364" t="s">
         <v>149</v>
       </c>
-      <c r="P7" s="338"/>
-      <c r="Q7" s="312" t="s">
+      <c r="P7" s="365"/>
+      <c r="Q7" s="339" t="s">
         <v>130</v>
       </c>
-      <c r="R7" s="313"/>
-      <c r="S7" s="309" t="s">
+      <c r="R7" s="340"/>
+      <c r="S7" s="336" t="s">
         <v>143</v>
       </c>
-      <c r="T7" s="310"/>
-      <c r="U7" s="311"/>
+      <c r="T7" s="337"/>
+      <c r="U7" s="338"/>
     </row>
     <row r="8" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
-      <c r="B8" s="288"/>
-      <c r="C8" s="301"/>
-      <c r="D8" s="302"/>
-      <c r="E8" s="303"/>
+      <c r="B8" s="390"/>
+      <c r="C8" s="400"/>
+      <c r="D8" s="401"/>
+      <c r="E8" s="402"/>
       <c r="F8" s="135"/>
       <c r="G8" s="146" t="s">
         <v>5</v>
@@ -3744,19 +3744,19 @@
         <f>input!D15</f>
         <v>0</v>
       </c>
-      <c r="M8" s="321"/>
+      <c r="M8" s="348"/>
       <c r="N8" s="138"/>
-      <c r="O8" s="339"/>
-      <c r="P8" s="340"/>
-      <c r="Q8" s="330" t="s">
+      <c r="O8" s="366"/>
+      <c r="P8" s="367"/>
+      <c r="Q8" s="357" t="s">
         <v>129</v>
       </c>
-      <c r="R8" s="363" t="s">
+      <c r="R8" s="298" t="s">
         <v>150</v>
       </c>
-      <c r="S8" s="272"/>
-      <c r="T8" s="274"/>
-      <c r="U8" s="276"/>
+      <c r="S8" s="376"/>
+      <c r="T8" s="378"/>
+      <c r="U8" s="380"/>
     </row>
     <row r="9" spans="2:31" ht="6" customHeight="1">
       <c r="B9" s="25"/>
@@ -3772,13 +3772,13 @@
       <c r="L9" s="44"/>
       <c r="M9" s="44"/>
       <c r="N9" s="33"/>
-      <c r="O9" s="339"/>
-      <c r="P9" s="340"/>
-      <c r="Q9" s="331"/>
-      <c r="R9" s="364"/>
-      <c r="S9" s="277"/>
-      <c r="T9" s="275"/>
-      <c r="U9" s="273"/>
+      <c r="O9" s="366"/>
+      <c r="P9" s="367"/>
+      <c r="Q9" s="358"/>
+      <c r="R9" s="299"/>
+      <c r="S9" s="381"/>
+      <c r="T9" s="379"/>
+      <c r="U9" s="377"/>
     </row>
     <row r="10" spans="2:31" ht="17.25" customHeight="1" thickBot="1">
       <c r="B10" s="34"/>
@@ -3794,24 +3794,24 @@
       <c r="L10" s="211"/>
       <c r="M10" s="44"/>
       <c r="N10" s="33"/>
-      <c r="O10" s="341"/>
-      <c r="P10" s="342"/>
-      <c r="Q10" s="332"/>
-      <c r="R10" s="365"/>
-      <c r="S10" s="278"/>
-      <c r="T10" s="279"/>
-      <c r="U10" s="280"/>
+      <c r="O10" s="368"/>
+      <c r="P10" s="369"/>
+      <c r="Q10" s="359"/>
+      <c r="R10" s="300"/>
+      <c r="S10" s="382"/>
+      <c r="T10" s="383"/>
+      <c r="U10" s="384"/>
     </row>
     <row r="11" spans="2:31" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B11" s="290" t="s">
+      <c r="B11" s="303" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="370" t="str">
+      <c r="C11" s="309" t="str">
         <f>IF(C13=0,"","DR"&amp;MID(C13,2,4))</f>
         <v/>
       </c>
-      <c r="D11" s="370"/>
-      <c r="E11" s="371"/>
+      <c r="D11" s="309"/>
+      <c r="E11" s="310"/>
       <c r="F11" s="44"/>
       <c r="G11" s="60" t="s">
         <v>128</v>
@@ -3823,21 +3823,21 @@
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="33"/>
-      <c r="O11" s="333"/>
-      <c r="P11" s="334"/>
-      <c r="Q11" s="357"/>
-      <c r="R11" s="360"/>
-      <c r="S11" s="354" t="s">
+      <c r="O11" s="360"/>
+      <c r="P11" s="361"/>
+      <c r="Q11" s="330"/>
+      <c r="R11" s="333"/>
+      <c r="S11" s="301" t="s">
         <v>85</v>
       </c>
-      <c r="T11" s="355"/>
-      <c r="U11" s="356"/>
+      <c r="T11" s="329"/>
+      <c r="U11" s="302"/>
     </row>
     <row r="12" spans="2:31" ht="26.25" customHeight="1">
-      <c r="B12" s="291"/>
-      <c r="C12" s="372"/>
-      <c r="D12" s="372"/>
-      <c r="E12" s="373"/>
+      <c r="B12" s="304"/>
+      <c r="C12" s="311"/>
+      <c r="D12" s="311"/>
+      <c r="E12" s="312"/>
       <c r="F12" s="25"/>
       <c r="G12" s="136" t="s">
         <v>135</v>
@@ -3849,24 +3849,24 @@
       <c r="L12" s="39"/>
       <c r="M12" s="40"/>
       <c r="N12" s="33"/>
-      <c r="O12" s="335"/>
-      <c r="P12" s="336"/>
-      <c r="Q12" s="358"/>
-      <c r="R12" s="361"/>
-      <c r="S12" s="281"/>
-      <c r="T12" s="282"/>
-      <c r="U12" s="283"/>
+      <c r="O12" s="362"/>
+      <c r="P12" s="363"/>
+      <c r="Q12" s="331"/>
+      <c r="R12" s="334"/>
+      <c r="S12" s="385"/>
+      <c r="T12" s="386"/>
+      <c r="U12" s="387"/>
     </row>
     <row r="13" spans="2:31" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B13" s="287" t="s">
+      <c r="B13" s="305" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="372">
+      <c r="C13" s="311">
         <f>input!D32</f>
         <v>0</v>
       </c>
-      <c r="D13" s="372"/>
-      <c r="E13" s="373"/>
+      <c r="D13" s="311"/>
+      <c r="E13" s="312"/>
       <c r="F13" s="25"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
@@ -3876,19 +3876,19 @@
       <c r="L13" s="44"/>
       <c r="M13" s="44"/>
       <c r="N13" s="33"/>
-      <c r="O13" s="325"/>
-      <c r="P13" s="327"/>
-      <c r="Q13" s="359"/>
-      <c r="R13" s="362"/>
-      <c r="S13" s="284"/>
-      <c r="T13" s="285"/>
-      <c r="U13" s="286"/>
+      <c r="O13" s="354"/>
+      <c r="P13" s="356"/>
+      <c r="Q13" s="332"/>
+      <c r="R13" s="335"/>
+      <c r="S13" s="306"/>
+      <c r="T13" s="388"/>
+      <c r="U13" s="389"/>
     </row>
     <row r="14" spans="2:31" ht="27" customHeight="1" thickBot="1">
-      <c r="B14" s="284"/>
-      <c r="C14" s="374"/>
-      <c r="D14" s="374"/>
-      <c r="E14" s="375"/>
+      <c r="B14" s="306"/>
+      <c r="C14" s="313"/>
+      <c r="D14" s="313"/>
+      <c r="E14" s="314"/>
       <c r="F14" s="44"/>
       <c r="G14" s="134" t="s">
         <v>6</v>
@@ -3900,17 +3900,17 @@
       <c r="L14" s="44"/>
       <c r="M14" s="44"/>
       <c r="N14" s="33"/>
-      <c r="O14" s="272" t="s">
+      <c r="O14" s="376" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="273"/>
-      <c r="Q14" s="272" t="s">
+      <c r="P14" s="377"/>
+      <c r="Q14" s="376" t="s">
         <v>151</v>
       </c>
-      <c r="R14" s="274"/>
-      <c r="S14" s="275"/>
-      <c r="T14" s="275"/>
-      <c r="U14" s="273"/>
+      <c r="R14" s="378"/>
+      <c r="S14" s="379"/>
+      <c r="T14" s="379"/>
+      <c r="U14" s="377"/>
     </row>
     <row r="15" spans="2:31" ht="52.5" customHeight="1" thickBot="1">
       <c r="B15" s="212" t="s">
@@ -3967,12 +3967,12 @@
       </c>
     </row>
     <row r="16" spans="2:31" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B16" s="376" t="s">
+      <c r="B16" s="315" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="377"/>
-      <c r="D16" s="378"/>
-      <c r="E16" s="356"/>
+      <c r="C16" s="316"/>
+      <c r="D16" s="317"/>
+      <c r="E16" s="302"/>
       <c r="F16" s="44"/>
       <c r="G16" s="132">
         <v>1</v>
@@ -4010,10 +4010,10 @@
       <c r="C17" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="368" t="s">
+      <c r="D17" s="307" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="369"/>
+      <c r="E17" s="308"/>
       <c r="F17" s="44"/>
       <c r="G17" s="132">
         <v>2</v>
@@ -4047,8 +4047,8 @@
     <row r="18" spans="2:31" ht="35.1" customHeight="1">
       <c r="B18" s="127"/>
       <c r="C18" s="45"/>
-      <c r="D18" s="366"/>
-      <c r="E18" s="367"/>
+      <c r="D18" s="280"/>
+      <c r="E18" s="281"/>
       <c r="F18" s="44"/>
       <c r="G18" s="132">
         <v>3</v>
@@ -4082,8 +4082,8 @@
     <row r="19" spans="2:31" ht="35.1" customHeight="1">
       <c r="B19" s="127"/>
       <c r="C19" s="45"/>
-      <c r="D19" s="366"/>
-      <c r="E19" s="367"/>
+      <c r="D19" s="280"/>
+      <c r="E19" s="281"/>
       <c r="F19" s="44"/>
       <c r="G19" s="132">
         <v>4</v>
@@ -4109,10 +4109,10 @@
       <c r="T19" s="47"/>
       <c r="U19" s="48"/>
       <c r="W19" s="49"/>
-      <c r="X19" s="352"/>
-      <c r="Y19" s="289"/>
-      <c r="Z19" s="289"/>
-      <c r="AA19" s="289"/>
+      <c r="X19" s="327"/>
+      <c r="Y19" s="320"/>
+      <c r="Z19" s="320"/>
+      <c r="AA19" s="320"/>
       <c r="AB19" s="44"/>
       <c r="AC19" s="44"/>
       <c r="AD19" s="44"/>
@@ -4121,8 +4121,8 @@
     <row r="20" spans="2:31" ht="35.1" customHeight="1">
       <c r="B20" s="127"/>
       <c r="C20" s="45"/>
-      <c r="D20" s="366"/>
-      <c r="E20" s="367"/>
+      <c r="D20" s="280"/>
+      <c r="E20" s="281"/>
       <c r="F20" s="44"/>
       <c r="G20" s="132">
         <v>5</v>
@@ -4146,8 +4146,8 @@
       <c r="W20" s="44"/>
       <c r="X20" s="129"/>
       <c r="Y20" s="43"/>
-      <c r="Z20" s="353"/>
-      <c r="AA20" s="289"/>
+      <c r="Z20" s="328"/>
+      <c r="AA20" s="320"/>
       <c r="AB20" s="44"/>
       <c r="AC20" s="44"/>
       <c r="AD20" s="44"/>
@@ -4156,8 +4156,8 @@
     <row r="21" spans="2:31" ht="35.1" customHeight="1">
       <c r="B21" s="127"/>
       <c r="C21" s="45"/>
-      <c r="D21" s="366"/>
-      <c r="E21" s="367"/>
+      <c r="D21" s="280"/>
+      <c r="E21" s="281"/>
       <c r="F21" s="44"/>
       <c r="G21" s="132">
         <v>6</v>
@@ -4182,8 +4182,8 @@
       <c r="W21" s="44"/>
       <c r="X21" s="129"/>
       <c r="Y21" s="130"/>
-      <c r="Z21" s="343"/>
-      <c r="AA21" s="289"/>
+      <c r="Z21" s="266"/>
+      <c r="AA21" s="320"/>
       <c r="AB21" s="44"/>
       <c r="AC21" s="44"/>
       <c r="AD21" s="44"/>
@@ -4192,8 +4192,8 @@
     <row r="22" spans="2:31" ht="35.1" customHeight="1">
       <c r="B22" s="127"/>
       <c r="C22" s="45"/>
-      <c r="D22" s="366"/>
-      <c r="E22" s="367"/>
+      <c r="D22" s="280"/>
+      <c r="E22" s="281"/>
       <c r="F22" s="44"/>
       <c r="G22" s="132">
         <v>7</v>
@@ -4218,8 +4218,8 @@
       <c r="W22" s="44"/>
       <c r="X22" s="43"/>
       <c r="Y22" s="44"/>
-      <c r="Z22" s="289"/>
-      <c r="AA22" s="289"/>
+      <c r="Z22" s="320"/>
+      <c r="AA22" s="320"/>
       <c r="AB22" s="44"/>
       <c r="AC22" s="44"/>
       <c r="AD22" s="44"/>
@@ -4228,8 +4228,8 @@
     <row r="23" spans="2:31" ht="35.1" customHeight="1">
       <c r="B23" s="127"/>
       <c r="C23" s="45"/>
-      <c r="D23" s="366"/>
-      <c r="E23" s="367"/>
+      <c r="D23" s="280"/>
+      <c r="E23" s="281"/>
       <c r="F23" s="44"/>
       <c r="G23" s="132">
         <v>8</v>
@@ -4264,8 +4264,8 @@
     <row r="24" spans="2:31" ht="35.1" customHeight="1" thickBot="1">
       <c r="B24" s="128"/>
       <c r="C24" s="30"/>
-      <c r="D24" s="386"/>
-      <c r="E24" s="387"/>
+      <c r="D24" s="278"/>
+      <c r="E24" s="279"/>
       <c r="F24" s="44"/>
       <c r="G24" s="132">
         <v>9</v>
@@ -4328,14 +4328,14 @@
       <c r="W25" s="50"/>
     </row>
     <row r="26" spans="2:31" ht="39.75" customHeight="1" thickBot="1">
-      <c r="B26" s="354" t="s">
+      <c r="B26" s="301" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="356"/>
-      <c r="D26" s="354" t="s">
+      <c r="C26" s="302"/>
+      <c r="D26" s="301" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="356"/>
+      <c r="E26" s="302"/>
       <c r="F26" s="44"/>
       <c r="G26" s="132">
         <v>11</v>
@@ -4774,10 +4774,10 @@
       <c r="U38" s="48"/>
     </row>
     <row r="39" spans="2:23" s="55" customFormat="1" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B39" s="384" t="s">
+      <c r="B39" s="276" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="385"/>
+      <c r="C39" s="277"/>
       <c r="D39" s="167"/>
       <c r="E39" s="125"/>
       <c r="F39" s="117"/>
@@ -4944,14 +4944,14 @@
       <c r="U44" s="48"/>
     </row>
     <row r="45" spans="2:23" s="55" customFormat="1" ht="35.1" customHeight="1">
-      <c r="B45" s="379" t="s">
+      <c r="B45" s="318" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="381" t="s">
+      <c r="C45" s="273" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="382"/>
-      <c r="E45" s="383"/>
+      <c r="D45" s="274"/>
+      <c r="E45" s="275"/>
       <c r="F45" s="117"/>
       <c r="G45" s="132">
         <v>30</v>
@@ -4974,7 +4974,7 @@
       <c r="U45" s="48"/>
     </row>
     <row r="46" spans="2:23" s="55" customFormat="1" ht="35.1" customHeight="1">
-      <c r="B46" s="380"/>
+      <c r="B46" s="319"/>
       <c r="C46" s="237" t="s">
         <v>97</v>
       </c>
@@ -5062,14 +5062,14 @@
       <c r="U48" s="48"/>
     </row>
     <row r="49" spans="2:25" ht="35.1" customHeight="1">
-      <c r="B49" s="379" t="s">
+      <c r="B49" s="318" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="381" t="s">
+      <c r="C49" s="273" t="s">
         <v>114</v>
       </c>
-      <c r="D49" s="382"/>
-      <c r="E49" s="383"/>
+      <c r="D49" s="274"/>
+      <c r="E49" s="275"/>
       <c r="F49" s="44"/>
       <c r="G49" s="132">
         <v>34</v>
@@ -5092,7 +5092,7 @@
       <c r="U49" s="48"/>
     </row>
     <row r="50" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B50" s="380"/>
+      <c r="B50" s="319"/>
       <c r="C50" s="237" t="s">
         <v>97</v>
       </c>
@@ -5150,10 +5150,10 @@
       <c r="S51" s="45"/>
       <c r="T51" s="47"/>
       <c r="U51" s="48"/>
-      <c r="X51" s="344" t="s">
+      <c r="X51" s="321" t="s">
         <v>26</v>
       </c>
-      <c r="Y51" s="345"/>
+      <c r="Y51" s="322"/>
     </row>
     <row r="52" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
       <c r="B52" s="177" t="s">
@@ -5218,12 +5218,12 @@
       <c r="Y53" s="52"/>
     </row>
     <row r="54" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B54" s="346" t="s">
+      <c r="B54" s="287" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="392"/>
-      <c r="D54" s="394"/>
-      <c r="E54" s="395"/>
+      <c r="C54" s="288"/>
+      <c r="D54" s="291"/>
+      <c r="E54" s="292"/>
       <c r="F54" s="240"/>
       <c r="G54" s="132">
         <v>39</v>
@@ -5250,12 +5250,12 @@
       <c r="Y54" s="32"/>
     </row>
     <row r="55" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B55" s="390" t="s">
+      <c r="B55" s="285" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="391"/>
-      <c r="D55" s="396"/>
-      <c r="E55" s="397"/>
+      <c r="C55" s="286"/>
+      <c r="D55" s="293"/>
+      <c r="E55" s="294"/>
       <c r="F55" s="240"/>
       <c r="G55" s="133">
         <v>40</v>
@@ -5278,12 +5278,12 @@
       <c r="U55" s="62"/>
     </row>
     <row r="56" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B56" s="348" t="s">
+      <c r="B56" s="289" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="393"/>
-      <c r="D56" s="307"/>
-      <c r="E56" s="388"/>
+      <c r="C56" s="290"/>
+      <c r="D56" s="282"/>
+      <c r="E56" s="283"/>
       <c r="F56" s="240"/>
       <c r="G56" s="238" t="s">
         <v>87</v>
@@ -5347,61 +5347,61 @@
       <c r="B58" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="C58" s="398"/>
-      <c r="D58" s="398"/>
-      <c r="E58" s="399"/>
-      <c r="F58" s="389"/>
-      <c r="G58" s="263" t="s">
+      <c r="C58" s="295"/>
+      <c r="D58" s="295"/>
+      <c r="E58" s="296"/>
+      <c r="F58" s="284"/>
+      <c r="G58" s="410" t="s">
         <v>136</v>
       </c>
-      <c r="H58" s="264"/>
-      <c r="I58" s="264"/>
-      <c r="J58" s="265"/>
-      <c r="K58" s="263" t="s">
+      <c r="H58" s="411"/>
+      <c r="I58" s="411"/>
+      <c r="J58" s="412"/>
+      <c r="K58" s="410" t="s">
         <v>146</v>
       </c>
-      <c r="L58" s="264"/>
-      <c r="M58" s="264"/>
-      <c r="N58" s="265"/>
+      <c r="L58" s="411"/>
+      <c r="M58" s="411"/>
+      <c r="N58" s="412"/>
       <c r="O58" s="253" t="s">
         <v>8</v>
       </c>
       <c r="P58" s="256" t="s">
         <v>155</v>
       </c>
-      <c r="Q58" s="259" t="s">
+      <c r="Q58" s="406" t="s">
         <v>148</v>
       </c>
-      <c r="R58" s="260"/>
-      <c r="S58" s="404" t="s">
+      <c r="R58" s="407"/>
+      <c r="S58" s="262" t="s">
         <v>152</v>
       </c>
-      <c r="T58" s="405"/>
-      <c r="U58" s="406"/>
+      <c r="T58" s="263"/>
+      <c r="U58" s="264"/>
     </row>
     <row r="59" spans="2:25" ht="28.5" customHeight="1">
       <c r="B59" s="25"/>
       <c r="C59" s="44"/>
       <c r="D59" s="44"/>
       <c r="E59" s="33"/>
-      <c r="F59" s="389"/>
+      <c r="F59" s="284"/>
       <c r="G59" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="H59" s="257" t="s">
+      <c r="H59" s="349" t="s">
         <v>138</v>
       </c>
-      <c r="I59" s="258"/>
+      <c r="I59" s="350"/>
       <c r="J59" s="182" t="s">
         <v>137</v>
       </c>
       <c r="K59" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="L59" s="257" t="s">
+      <c r="L59" s="349" t="s">
         <v>138</v>
       </c>
-      <c r="M59" s="258"/>
+      <c r="M59" s="350"/>
       <c r="N59" s="239" t="s">
         <v>137</v>
       </c>
@@ -5409,11 +5409,11 @@
         <v>1</v>
       </c>
       <c r="P59" s="255"/>
-      <c r="Q59" s="261"/>
-      <c r="R59" s="262"/>
-      <c r="S59" s="407"/>
-      <c r="T59" s="343"/>
-      <c r="U59" s="408"/>
+      <c r="Q59" s="408"/>
+      <c r="R59" s="409"/>
+      <c r="S59" s="265"/>
+      <c r="T59" s="266"/>
+      <c r="U59" s="267"/>
     </row>
     <row r="60" spans="2:25" ht="28.5" customHeight="1">
       <c r="B60" s="25"/>
@@ -5424,24 +5424,24 @@
       <c r="G60" s="183">
         <v>1</v>
       </c>
-      <c r="H60" s="328"/>
-      <c r="I60" s="329"/>
+      <c r="H60" s="271"/>
+      <c r="I60" s="272"/>
       <c r="J60" s="184"/>
       <c r="K60" s="183">
         <v>1</v>
       </c>
-      <c r="L60" s="328"/>
-      <c r="M60" s="329"/>
+      <c r="L60" s="271"/>
+      <c r="M60" s="272"/>
       <c r="N60" s="221"/>
       <c r="O60" s="65">
         <v>2</v>
       </c>
       <c r="P60" s="222"/>
-      <c r="Q60" s="400"/>
-      <c r="R60" s="401"/>
-      <c r="S60" s="407"/>
-      <c r="T60" s="343"/>
-      <c r="U60" s="408"/>
+      <c r="Q60" s="258"/>
+      <c r="R60" s="259"/>
+      <c r="S60" s="265"/>
+      <c r="T60" s="266"/>
+      <c r="U60" s="267"/>
     </row>
     <row r="61" spans="2:25" ht="28.5" customHeight="1">
       <c r="B61" s="25"/>
@@ -5452,24 +5452,24 @@
       <c r="G61" s="183">
         <v>2</v>
       </c>
-      <c r="H61" s="328"/>
-      <c r="I61" s="329"/>
+      <c r="H61" s="271"/>
+      <c r="I61" s="272"/>
       <c r="J61" s="184"/>
       <c r="K61" s="183">
         <v>2</v>
       </c>
-      <c r="L61" s="328"/>
-      <c r="M61" s="329"/>
+      <c r="L61" s="271"/>
+      <c r="M61" s="272"/>
       <c r="N61" s="221"/>
       <c r="O61" s="65">
         <v>3</v>
       </c>
       <c r="P61" s="222"/>
-      <c r="Q61" s="400"/>
-      <c r="R61" s="401"/>
-      <c r="S61" s="407"/>
-      <c r="T61" s="343"/>
-      <c r="U61" s="408"/>
+      <c r="Q61" s="258"/>
+      <c r="R61" s="259"/>
+      <c r="S61" s="265"/>
+      <c r="T61" s="266"/>
+      <c r="U61" s="267"/>
     </row>
     <row r="62" spans="2:25" ht="28.5" customHeight="1">
       <c r="B62" s="25"/>
@@ -5480,24 +5480,24 @@
       <c r="G62" s="183">
         <v>3</v>
       </c>
-      <c r="H62" s="328"/>
-      <c r="I62" s="329"/>
+      <c r="H62" s="271"/>
+      <c r="I62" s="272"/>
       <c r="J62" s="184"/>
       <c r="K62" s="183">
         <v>3</v>
       </c>
-      <c r="L62" s="328"/>
-      <c r="M62" s="329"/>
+      <c r="L62" s="271"/>
+      <c r="M62" s="272"/>
       <c r="N62" s="221"/>
       <c r="O62" s="65">
         <v>4</v>
       </c>
       <c r="P62" s="222"/>
-      <c r="Q62" s="400"/>
-      <c r="R62" s="401"/>
-      <c r="S62" s="407"/>
-      <c r="T62" s="343"/>
-      <c r="U62" s="408"/>
+      <c r="Q62" s="258"/>
+      <c r="R62" s="259"/>
+      <c r="S62" s="265"/>
+      <c r="T62" s="266"/>
+      <c r="U62" s="267"/>
     </row>
     <row r="63" spans="2:25" ht="28.5" customHeight="1">
       <c r="B63" s="25"/>
@@ -5508,24 +5508,24 @@
       <c r="G63" s="183">
         <v>4</v>
       </c>
-      <c r="H63" s="328"/>
-      <c r="I63" s="329"/>
+      <c r="H63" s="271"/>
+      <c r="I63" s="272"/>
       <c r="J63" s="184"/>
       <c r="K63" s="183">
         <v>4</v>
       </c>
-      <c r="L63" s="328"/>
-      <c r="M63" s="329"/>
+      <c r="L63" s="271"/>
+      <c r="M63" s="272"/>
       <c r="N63" s="221"/>
       <c r="O63" s="65">
         <v>5</v>
       </c>
       <c r="P63" s="222"/>
-      <c r="Q63" s="400"/>
-      <c r="R63" s="401"/>
-      <c r="S63" s="407"/>
-      <c r="T63" s="343"/>
-      <c r="U63" s="408"/>
+      <c r="Q63" s="258"/>
+      <c r="R63" s="259"/>
+      <c r="S63" s="265"/>
+      <c r="T63" s="266"/>
+      <c r="U63" s="267"/>
     </row>
     <row r="64" spans="2:25" ht="28.5" customHeight="1">
       <c r="B64" s="25"/>
@@ -5536,24 +5536,24 @@
       <c r="G64" s="183">
         <v>5</v>
       </c>
-      <c r="H64" s="328"/>
-      <c r="I64" s="329"/>
+      <c r="H64" s="271"/>
+      <c r="I64" s="272"/>
       <c r="J64" s="184"/>
       <c r="K64" s="183">
         <v>5</v>
       </c>
-      <c r="L64" s="328"/>
-      <c r="M64" s="329"/>
+      <c r="L64" s="271"/>
+      <c r="M64" s="272"/>
       <c r="N64" s="221"/>
       <c r="O64" s="65">
         <v>6</v>
       </c>
       <c r="P64" s="222"/>
-      <c r="Q64" s="400"/>
-      <c r="R64" s="401"/>
-      <c r="S64" s="407"/>
-      <c r="T64" s="343"/>
-      <c r="U64" s="408"/>
+      <c r="Q64" s="258"/>
+      <c r="R64" s="259"/>
+      <c r="S64" s="265"/>
+      <c r="T64" s="266"/>
+      <c r="U64" s="267"/>
     </row>
     <row r="65" spans="2:35" ht="28.5" customHeight="1">
       <c r="B65" s="25"/>
@@ -5564,24 +5564,24 @@
       <c r="G65" s="183">
         <v>6</v>
       </c>
-      <c r="H65" s="328"/>
-      <c r="I65" s="329"/>
+      <c r="H65" s="271"/>
+      <c r="I65" s="272"/>
       <c r="J65" s="184"/>
       <c r="K65" s="183">
         <v>6</v>
       </c>
-      <c r="L65" s="328"/>
-      <c r="M65" s="329"/>
+      <c r="L65" s="271"/>
+      <c r="M65" s="272"/>
       <c r="N65" s="221"/>
       <c r="O65" s="65">
         <v>7</v>
       </c>
       <c r="P65" s="222"/>
-      <c r="Q65" s="400"/>
-      <c r="R65" s="401"/>
-      <c r="S65" s="407"/>
-      <c r="T65" s="343"/>
-      <c r="U65" s="408"/>
+      <c r="Q65" s="258"/>
+      <c r="R65" s="259"/>
+      <c r="S65" s="265"/>
+      <c r="T65" s="266"/>
+      <c r="U65" s="267"/>
     </row>
     <row r="66" spans="2:35" ht="28.5" customHeight="1" thickBot="1">
       <c r="B66" s="207"/>
@@ -5592,24 +5592,24 @@
       <c r="G66" s="236">
         <v>7</v>
       </c>
-      <c r="H66" s="307"/>
-      <c r="I66" s="308"/>
+      <c r="H66" s="282"/>
+      <c r="I66" s="297"/>
       <c r="J66" s="242"/>
       <c r="K66" s="236">
         <v>7</v>
       </c>
-      <c r="L66" s="307"/>
-      <c r="M66" s="308"/>
+      <c r="L66" s="282"/>
+      <c r="M66" s="297"/>
       <c r="N66" s="150"/>
       <c r="O66" s="66">
         <v>8</v>
       </c>
       <c r="P66" s="223"/>
-      <c r="Q66" s="402"/>
-      <c r="R66" s="403"/>
-      <c r="S66" s="409"/>
-      <c r="T66" s="410"/>
-      <c r="U66" s="411"/>
+      <c r="Q66" s="260"/>
+      <c r="R66" s="261"/>
+      <c r="S66" s="268"/>
+      <c r="T66" s="269"/>
+      <c r="U66" s="270"/>
     </row>
     <row r="67" spans="2:35" ht="21.95" customHeight="1">
       <c r="B67" s="219"/>
@@ -7687,14 +7687,77 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="Q66:R66"/>
-    <mergeCell ref="S58:U66"/>
-    <mergeCell ref="Q60:R60"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="Q59:R59"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="S8:U10"/>
+    <mergeCell ref="S12:U13"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="Q5:U6"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="Q8:Q10"/>
+    <mergeCell ref="O11:P13"/>
+    <mergeCell ref="O7:P10"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="L62:M62"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="Z21:AA22"/>
+    <mergeCell ref="X51:Y51"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="X19:AA19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H65:I65"/>
     <mergeCell ref="H60:I60"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="B39:C39"/>
@@ -7711,77 +7774,14 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="C58:E58"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="L63:M63"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="Z21:AA22"/>
-    <mergeCell ref="X51:Y51"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="X19:AA19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="Q5:U6"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="Q8:Q10"/>
-    <mergeCell ref="O11:P13"/>
-    <mergeCell ref="O7:P10"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="L62:M62"/>
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="S8:U10"/>
-    <mergeCell ref="S12:U13"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="Q59:R59"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="Q65:R65"/>
+    <mergeCell ref="Q66:R66"/>
+    <mergeCell ref="S58:U66"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="Q64:R64"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0" top="0" bottom="7.874015748031496E-2" header="0" footer="0"/>

</xml_diff>

<commit_message>
Change SQL, php of DieStatusV2
</commit_message>
<xml_diff>
--- a/py/direction_sheet.xlsx
+++ b/py/direction_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\diereport\ex0.11\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8885CBE7-90A9-4071-B01B-D1C379416122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31F52E0-9D0B-4B59-A71F-AD8512A0062A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="12420" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="print" sheetId="1" r:id="rId1"/>
@@ -2567,6 +2567,423 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="79" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2591,9 +3008,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2605,420 +3019,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="79" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3440,7 +3440,7 @@
   <dimension ref="B1:AI162"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:U1"/>
+      <selection activeCell="M5" sqref="M5:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="20.25"/>
@@ -3469,28 +3469,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="66.75" customHeight="1" thickBot="1">
-      <c r="B1" s="370" t="s">
+      <c r="B1" s="267" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="371"/>
-      <c r="D1" s="371"/>
-      <c r="E1" s="371"/>
-      <c r="F1" s="372"/>
-      <c r="G1" s="372"/>
-      <c r="H1" s="372"/>
-      <c r="I1" s="372"/>
-      <c r="J1" s="372"/>
-      <c r="K1" s="372"/>
-      <c r="L1" s="372"/>
-      <c r="M1" s="372"/>
-      <c r="N1" s="372"/>
-      <c r="O1" s="371"/>
-      <c r="P1" s="371"/>
-      <c r="Q1" s="371"/>
-      <c r="R1" s="371"/>
-      <c r="S1" s="371"/>
-      <c r="T1" s="371"/>
-      <c r="U1" s="373"/>
+      <c r="C1" s="268"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
+      <c r="F1" s="269"/>
+      <c r="G1" s="269"/>
+      <c r="H1" s="269"/>
+      <c r="I1" s="269"/>
+      <c r="J1" s="269"/>
+      <c r="K1" s="269"/>
+      <c r="L1" s="269"/>
+      <c r="M1" s="269"/>
+      <c r="N1" s="269"/>
+      <c r="O1" s="268"/>
+      <c r="P1" s="268"/>
+      <c r="Q1" s="268"/>
+      <c r="R1" s="268"/>
+      <c r="S1" s="268"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="270"/>
     </row>
     <row r="2" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
       <c r="B2" s="252" t="s">
@@ -3507,26 +3507,26 @@
         <f>input!D8</f>
         <v>0</v>
       </c>
-      <c r="F2" s="374"/>
-      <c r="G2" s="375"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="272"/>
       <c r="H2" s="240"/>
       <c r="I2" s="139"/>
       <c r="J2" s="240"/>
       <c r="K2" s="140"/>
-      <c r="L2" s="375"/>
-      <c r="M2" s="320"/>
+      <c r="L2" s="272"/>
+      <c r="M2" s="290"/>
       <c r="N2" s="141"/>
-      <c r="O2" s="287" t="s">
+      <c r="O2" s="347" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="323"/>
-      <c r="Q2" s="287" t="s">
+      <c r="P2" s="348"/>
+      <c r="Q2" s="347" t="s">
         <v>125</v>
       </c>
-      <c r="R2" s="325"/>
-      <c r="S2" s="325"/>
-      <c r="T2" s="325"/>
-      <c r="U2" s="323"/>
+      <c r="R2" s="351"/>
+      <c r="S2" s="351"/>
+      <c r="T2" s="351"/>
+      <c r="U2" s="348"/>
     </row>
     <row r="3" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
       <c r="B3" s="236" t="s">
@@ -3543,24 +3543,24 @@
         <f>input!D9</f>
         <v>0</v>
       </c>
-      <c r="F3" s="374"/>
-      <c r="G3" s="375"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="272"/>
       <c r="H3" s="240"/>
       <c r="I3" s="140"/>
       <c r="J3" s="240"/>
       <c r="K3" s="44"/>
-      <c r="L3" s="375"/>
-      <c r="M3" s="320"/>
+      <c r="L3" s="272"/>
+      <c r="M3" s="290"/>
       <c r="N3" s="141"/>
-      <c r="O3" s="289" t="s">
+      <c r="O3" s="349" t="s">
         <v>131</v>
       </c>
-      <c r="P3" s="324"/>
-      <c r="Q3" s="289"/>
-      <c r="R3" s="326"/>
-      <c r="S3" s="326"/>
-      <c r="T3" s="326"/>
-      <c r="U3" s="324"/>
+      <c r="P3" s="350"/>
+      <c r="Q3" s="349"/>
+      <c r="R3" s="352"/>
+      <c r="S3" s="352"/>
+      <c r="T3" s="352"/>
+      <c r="U3" s="350"/>
     </row>
     <row r="4" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
       <c r="B4" s="25"/>
@@ -3568,17 +3568,17 @@
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
       <c r="F4" s="210"/>
-      <c r="G4" s="403" t="s">
+      <c r="G4" s="305" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="404"/>
-      <c r="I4" s="404"/>
-      <c r="J4" s="405"/>
-      <c r="K4" s="403" t="s">
+      <c r="H4" s="306"/>
+      <c r="I4" s="306"/>
+      <c r="J4" s="307"/>
+      <c r="K4" s="305" t="s">
         <v>142</v>
       </c>
-      <c r="L4" s="404"/>
-      <c r="M4" s="405"/>
+      <c r="L4" s="306"/>
+      <c r="M4" s="307"/>
       <c r="N4" s="143"/>
       <c r="O4" s="200" t="s">
         <v>83</v>
@@ -3586,24 +3586,24 @@
       <c r="P4" s="201" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="287" t="s">
+      <c r="Q4" s="347" t="s">
         <v>126</v>
       </c>
-      <c r="R4" s="325"/>
-      <c r="S4" s="325"/>
-      <c r="T4" s="325"/>
-      <c r="U4" s="323"/>
+      <c r="R4" s="351"/>
+      <c r="S4" s="351"/>
+      <c r="T4" s="351"/>
+      <c r="U4" s="348"/>
     </row>
     <row r="5" spans="2:31" ht="28.5" customHeight="1">
-      <c r="B5" s="303" t="s">
+      <c r="B5" s="291" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="391">
+      <c r="C5" s="293">
         <f>input!D6</f>
         <v>0</v>
       </c>
-      <c r="D5" s="392"/>
-      <c r="E5" s="393"/>
+      <c r="D5" s="294"/>
+      <c r="E5" s="295"/>
       <c r="F5" s="135"/>
       <c r="G5" s="145" t="s">
         <v>2</v>
@@ -3624,23 +3624,23 @@
       <c r="L5" s="193" t="s">
         <v>102</v>
       </c>
-      <c r="M5" s="345" t="s">
+      <c r="M5" s="319" t="s">
         <v>133</v>
       </c>
       <c r="N5" s="135"/>
-      <c r="O5" s="341"/>
-      <c r="P5" s="343"/>
-      <c r="Q5" s="351"/>
-      <c r="R5" s="352"/>
-      <c r="S5" s="352"/>
-      <c r="T5" s="352"/>
-      <c r="U5" s="353"/>
+      <c r="O5" s="315"/>
+      <c r="P5" s="317"/>
+      <c r="Q5" s="323"/>
+      <c r="R5" s="324"/>
+      <c r="S5" s="324"/>
+      <c r="T5" s="324"/>
+      <c r="U5" s="325"/>
     </row>
     <row r="6" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
-      <c r="B6" s="304"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="395"/>
-      <c r="E6" s="396"/>
+      <c r="B6" s="292"/>
+      <c r="C6" s="296"/>
+      <c r="D6" s="297"/>
+      <c r="E6" s="298"/>
       <c r="F6" s="135"/>
       <c r="G6" s="187">
         <v>6061</v>
@@ -3662,26 +3662,26 @@
         <f>ROUND(input!D14,2)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="346"/>
+      <c r="M6" s="320"/>
       <c r="N6" s="137"/>
-      <c r="O6" s="342"/>
-      <c r="P6" s="344"/>
-      <c r="Q6" s="354"/>
-      <c r="R6" s="355"/>
-      <c r="S6" s="355"/>
-      <c r="T6" s="355"/>
-      <c r="U6" s="356"/>
+      <c r="O6" s="316"/>
+      <c r="P6" s="318"/>
+      <c r="Q6" s="326"/>
+      <c r="R6" s="327"/>
+      <c r="S6" s="327"/>
+      <c r="T6" s="327"/>
+      <c r="U6" s="328"/>
     </row>
     <row r="7" spans="2:31" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B7" s="305" t="s">
+      <c r="B7" s="288" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="397">
+      <c r="C7" s="299">
         <f>input!D7</f>
         <v>0</v>
       </c>
-      <c r="D7" s="398"/>
-      <c r="E7" s="399"/>
+      <c r="D7" s="300"/>
+      <c r="E7" s="301"/>
       <c r="F7" s="135"/>
       <c r="G7" s="187">
         <v>6063</v>
@@ -3702,30 +3702,30 @@
       <c r="L7" s="197" t="s">
         <v>104</v>
       </c>
-      <c r="M7" s="347">
-        <f>input!D11</f>
+      <c r="M7" s="321">
+        <f>input!K11</f>
         <v>0</v>
       </c>
       <c r="N7" s="138"/>
-      <c r="O7" s="364" t="s">
+      <c r="O7" s="338" t="s">
         <v>149</v>
       </c>
-      <c r="P7" s="365"/>
-      <c r="Q7" s="339" t="s">
+      <c r="P7" s="339"/>
+      <c r="Q7" s="313" t="s">
         <v>130</v>
       </c>
-      <c r="R7" s="340"/>
-      <c r="S7" s="336" t="s">
+      <c r="R7" s="314"/>
+      <c r="S7" s="310" t="s">
         <v>143</v>
       </c>
-      <c r="T7" s="337"/>
-      <c r="U7" s="338"/>
+      <c r="T7" s="311"/>
+      <c r="U7" s="312"/>
     </row>
     <row r="8" spans="2:31" ht="28.5" customHeight="1" thickBot="1">
-      <c r="B8" s="390"/>
-      <c r="C8" s="400"/>
-      <c r="D8" s="401"/>
-      <c r="E8" s="402"/>
+      <c r="B8" s="289"/>
+      <c r="C8" s="302"/>
+      <c r="D8" s="303"/>
+      <c r="E8" s="304"/>
       <c r="F8" s="135"/>
       <c r="G8" s="146" t="s">
         <v>5</v>
@@ -3744,19 +3744,19 @@
         <f>input!D15</f>
         <v>0</v>
       </c>
-      <c r="M8" s="348"/>
+      <c r="M8" s="322"/>
       <c r="N8" s="138"/>
-      <c r="O8" s="366"/>
-      <c r="P8" s="367"/>
-      <c r="Q8" s="357" t="s">
+      <c r="O8" s="340"/>
+      <c r="P8" s="341"/>
+      <c r="Q8" s="331" t="s">
         <v>129</v>
       </c>
-      <c r="R8" s="298" t="s">
+      <c r="R8" s="364" t="s">
         <v>150</v>
       </c>
-      <c r="S8" s="376"/>
-      <c r="T8" s="378"/>
-      <c r="U8" s="380"/>
+      <c r="S8" s="273"/>
+      <c r="T8" s="275"/>
+      <c r="U8" s="277"/>
     </row>
     <row r="9" spans="2:31" ht="6" customHeight="1">
       <c r="B9" s="25"/>
@@ -3772,13 +3772,13 @@
       <c r="L9" s="44"/>
       <c r="M9" s="44"/>
       <c r="N9" s="33"/>
-      <c r="O9" s="366"/>
-      <c r="P9" s="367"/>
-      <c r="Q9" s="358"/>
-      <c r="R9" s="299"/>
-      <c r="S9" s="381"/>
-      <c r="T9" s="379"/>
-      <c r="U9" s="377"/>
+      <c r="O9" s="340"/>
+      <c r="P9" s="341"/>
+      <c r="Q9" s="332"/>
+      <c r="R9" s="365"/>
+      <c r="S9" s="278"/>
+      <c r="T9" s="276"/>
+      <c r="U9" s="274"/>
     </row>
     <row r="10" spans="2:31" ht="17.25" customHeight="1" thickBot="1">
       <c r="B10" s="34"/>
@@ -3794,24 +3794,24 @@
       <c r="L10" s="211"/>
       <c r="M10" s="44"/>
       <c r="N10" s="33"/>
-      <c r="O10" s="368"/>
-      <c r="P10" s="369"/>
-      <c r="Q10" s="359"/>
-      <c r="R10" s="300"/>
-      <c r="S10" s="382"/>
-      <c r="T10" s="383"/>
-      <c r="U10" s="384"/>
+      <c r="O10" s="342"/>
+      <c r="P10" s="343"/>
+      <c r="Q10" s="333"/>
+      <c r="R10" s="366"/>
+      <c r="S10" s="279"/>
+      <c r="T10" s="280"/>
+      <c r="U10" s="281"/>
     </row>
     <row r="11" spans="2:31" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B11" s="303" t="s">
+      <c r="B11" s="291" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="309" t="str">
+      <c r="C11" s="371" t="str">
         <f>IF(C13=0,"","DR"&amp;MID(C13,2,4))</f>
         <v/>
       </c>
-      <c r="D11" s="309"/>
-      <c r="E11" s="310"/>
+      <c r="D11" s="371"/>
+      <c r="E11" s="372"/>
       <c r="F11" s="44"/>
       <c r="G11" s="60" t="s">
         <v>128</v>
@@ -3823,21 +3823,21 @@
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="33"/>
-      <c r="O11" s="360"/>
-      <c r="P11" s="361"/>
-      <c r="Q11" s="330"/>
-      <c r="R11" s="333"/>
-      <c r="S11" s="301" t="s">
+      <c r="O11" s="334"/>
+      <c r="P11" s="335"/>
+      <c r="Q11" s="358"/>
+      <c r="R11" s="361"/>
+      <c r="S11" s="355" t="s">
         <v>85</v>
       </c>
-      <c r="T11" s="329"/>
-      <c r="U11" s="302"/>
+      <c r="T11" s="356"/>
+      <c r="U11" s="357"/>
     </row>
     <row r="12" spans="2:31" ht="26.25" customHeight="1">
-      <c r="B12" s="304"/>
-      <c r="C12" s="311"/>
-      <c r="D12" s="311"/>
-      <c r="E12" s="312"/>
+      <c r="B12" s="292"/>
+      <c r="C12" s="373"/>
+      <c r="D12" s="373"/>
+      <c r="E12" s="374"/>
       <c r="F12" s="25"/>
       <c r="G12" s="136" t="s">
         <v>135</v>
@@ -3849,24 +3849,24 @@
       <c r="L12" s="39"/>
       <c r="M12" s="40"/>
       <c r="N12" s="33"/>
-      <c r="O12" s="362"/>
-      <c r="P12" s="363"/>
-      <c r="Q12" s="331"/>
-      <c r="R12" s="334"/>
-      <c r="S12" s="385"/>
-      <c r="T12" s="386"/>
-      <c r="U12" s="387"/>
+      <c r="O12" s="336"/>
+      <c r="P12" s="337"/>
+      <c r="Q12" s="359"/>
+      <c r="R12" s="362"/>
+      <c r="S12" s="282"/>
+      <c r="T12" s="283"/>
+      <c r="U12" s="284"/>
     </row>
     <row r="13" spans="2:31" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B13" s="305" t="s">
+      <c r="B13" s="288" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="311">
+      <c r="C13" s="373">
         <f>input!D32</f>
         <v>0</v>
       </c>
-      <c r="D13" s="311"/>
-      <c r="E13" s="312"/>
+      <c r="D13" s="373"/>
+      <c r="E13" s="374"/>
       <c r="F13" s="25"/>
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
@@ -3876,19 +3876,19 @@
       <c r="L13" s="44"/>
       <c r="M13" s="44"/>
       <c r="N13" s="33"/>
-      <c r="O13" s="354"/>
-      <c r="P13" s="356"/>
-      <c r="Q13" s="332"/>
-      <c r="R13" s="335"/>
-      <c r="S13" s="306"/>
-      <c r="T13" s="388"/>
-      <c r="U13" s="389"/>
+      <c r="O13" s="326"/>
+      <c r="P13" s="328"/>
+      <c r="Q13" s="360"/>
+      <c r="R13" s="363"/>
+      <c r="S13" s="285"/>
+      <c r="T13" s="286"/>
+      <c r="U13" s="287"/>
     </row>
     <row r="14" spans="2:31" ht="27" customHeight="1" thickBot="1">
-      <c r="B14" s="306"/>
-      <c r="C14" s="313"/>
-      <c r="D14" s="313"/>
-      <c r="E14" s="314"/>
+      <c r="B14" s="285"/>
+      <c r="C14" s="375"/>
+      <c r="D14" s="375"/>
+      <c r="E14" s="376"/>
       <c r="F14" s="44"/>
       <c r="G14" s="134" t="s">
         <v>6</v>
@@ -3900,17 +3900,17 @@
       <c r="L14" s="44"/>
       <c r="M14" s="44"/>
       <c r="N14" s="33"/>
-      <c r="O14" s="376" t="s">
+      <c r="O14" s="273" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="377"/>
-      <c r="Q14" s="376" t="s">
+      <c r="P14" s="274"/>
+      <c r="Q14" s="273" t="s">
         <v>151</v>
       </c>
-      <c r="R14" s="378"/>
-      <c r="S14" s="379"/>
-      <c r="T14" s="379"/>
-      <c r="U14" s="377"/>
+      <c r="R14" s="275"/>
+      <c r="S14" s="276"/>
+      <c r="T14" s="276"/>
+      <c r="U14" s="274"/>
     </row>
     <row r="15" spans="2:31" ht="52.5" customHeight="1" thickBot="1">
       <c r="B15" s="212" t="s">
@@ -3967,12 +3967,12 @@
       </c>
     </row>
     <row r="16" spans="2:31" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B16" s="315" t="s">
+      <c r="B16" s="377" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="316"/>
-      <c r="D16" s="317"/>
-      <c r="E16" s="302"/>
+      <c r="C16" s="378"/>
+      <c r="D16" s="379"/>
+      <c r="E16" s="357"/>
       <c r="F16" s="44"/>
       <c r="G16" s="132">
         <v>1</v>
@@ -4010,10 +4010,10 @@
       <c r="C17" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="307" t="s">
+      <c r="D17" s="369" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="308"/>
+      <c r="E17" s="370"/>
       <c r="F17" s="44"/>
       <c r="G17" s="132">
         <v>2</v>
@@ -4047,8 +4047,8 @@
     <row r="18" spans="2:31" ht="35.1" customHeight="1">
       <c r="B18" s="127"/>
       <c r="C18" s="45"/>
-      <c r="D18" s="280"/>
-      <c r="E18" s="281"/>
+      <c r="D18" s="367"/>
+      <c r="E18" s="368"/>
       <c r="F18" s="44"/>
       <c r="G18" s="132">
         <v>3</v>
@@ -4082,8 +4082,8 @@
     <row r="19" spans="2:31" ht="35.1" customHeight="1">
       <c r="B19" s="127"/>
       <c r="C19" s="45"/>
-      <c r="D19" s="280"/>
-      <c r="E19" s="281"/>
+      <c r="D19" s="367"/>
+      <c r="E19" s="368"/>
       <c r="F19" s="44"/>
       <c r="G19" s="132">
         <v>4</v>
@@ -4109,10 +4109,10 @@
       <c r="T19" s="47"/>
       <c r="U19" s="48"/>
       <c r="W19" s="49"/>
-      <c r="X19" s="327"/>
-      <c r="Y19" s="320"/>
-      <c r="Z19" s="320"/>
-      <c r="AA19" s="320"/>
+      <c r="X19" s="353"/>
+      <c r="Y19" s="290"/>
+      <c r="Z19" s="290"/>
+      <c r="AA19" s="290"/>
       <c r="AB19" s="44"/>
       <c r="AC19" s="44"/>
       <c r="AD19" s="44"/>
@@ -4121,8 +4121,8 @@
     <row r="20" spans="2:31" ht="35.1" customHeight="1">
       <c r="B20" s="127"/>
       <c r="C20" s="45"/>
-      <c r="D20" s="280"/>
-      <c r="E20" s="281"/>
+      <c r="D20" s="367"/>
+      <c r="E20" s="368"/>
       <c r="F20" s="44"/>
       <c r="G20" s="132">
         <v>5</v>
@@ -4146,8 +4146,8 @@
       <c r="W20" s="44"/>
       <c r="X20" s="129"/>
       <c r="Y20" s="43"/>
-      <c r="Z20" s="328"/>
-      <c r="AA20" s="320"/>
+      <c r="Z20" s="354"/>
+      <c r="AA20" s="290"/>
       <c r="AB20" s="44"/>
       <c r="AC20" s="44"/>
       <c r="AD20" s="44"/>
@@ -4156,8 +4156,8 @@
     <row r="21" spans="2:31" ht="35.1" customHeight="1">
       <c r="B21" s="127"/>
       <c r="C21" s="45"/>
-      <c r="D21" s="280"/>
-      <c r="E21" s="281"/>
+      <c r="D21" s="367"/>
+      <c r="E21" s="368"/>
       <c r="F21" s="44"/>
       <c r="G21" s="132">
         <v>6</v>
@@ -4182,8 +4182,8 @@
       <c r="W21" s="44"/>
       <c r="X21" s="129"/>
       <c r="Y21" s="130"/>
-      <c r="Z21" s="266"/>
-      <c r="AA21" s="320"/>
+      <c r="Z21" s="344"/>
+      <c r="AA21" s="290"/>
       <c r="AB21" s="44"/>
       <c r="AC21" s="44"/>
       <c r="AD21" s="44"/>
@@ -4192,8 +4192,8 @@
     <row r="22" spans="2:31" ht="35.1" customHeight="1">
       <c r="B22" s="127"/>
       <c r="C22" s="45"/>
-      <c r="D22" s="280"/>
-      <c r="E22" s="281"/>
+      <c r="D22" s="367"/>
+      <c r="E22" s="368"/>
       <c r="F22" s="44"/>
       <c r="G22" s="132">
         <v>7</v>
@@ -4218,8 +4218,8 @@
       <c r="W22" s="44"/>
       <c r="X22" s="43"/>
       <c r="Y22" s="44"/>
-      <c r="Z22" s="320"/>
-      <c r="AA22" s="320"/>
+      <c r="Z22" s="290"/>
+      <c r="AA22" s="290"/>
       <c r="AB22" s="44"/>
       <c r="AC22" s="44"/>
       <c r="AD22" s="44"/>
@@ -4228,8 +4228,8 @@
     <row r="23" spans="2:31" ht="35.1" customHeight="1">
       <c r="B23" s="127"/>
       <c r="C23" s="45"/>
-      <c r="D23" s="280"/>
-      <c r="E23" s="281"/>
+      <c r="D23" s="367"/>
+      <c r="E23" s="368"/>
       <c r="F23" s="44"/>
       <c r="G23" s="132">
         <v>8</v>
@@ -4264,8 +4264,8 @@
     <row r="24" spans="2:31" ht="35.1" customHeight="1" thickBot="1">
       <c r="B24" s="128"/>
       <c r="C24" s="30"/>
-      <c r="D24" s="278"/>
-      <c r="E24" s="279"/>
+      <c r="D24" s="387"/>
+      <c r="E24" s="388"/>
       <c r="F24" s="44"/>
       <c r="G24" s="132">
         <v>9</v>
@@ -4328,14 +4328,14 @@
       <c r="W25" s="50"/>
     </row>
     <row r="26" spans="2:31" ht="39.75" customHeight="1" thickBot="1">
-      <c r="B26" s="301" t="s">
+      <c r="B26" s="355" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="302"/>
-      <c r="D26" s="301" t="s">
+      <c r="C26" s="357"/>
+      <c r="D26" s="355" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="302"/>
+      <c r="E26" s="357"/>
       <c r="F26" s="44"/>
       <c r="G26" s="132">
         <v>11</v>
@@ -4774,10 +4774,10 @@
       <c r="U38" s="48"/>
     </row>
     <row r="39" spans="2:23" s="55" customFormat="1" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B39" s="276" t="s">
+      <c r="B39" s="385" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="277"/>
+      <c r="C39" s="386"/>
       <c r="D39" s="167"/>
       <c r="E39" s="125"/>
       <c r="F39" s="117"/>
@@ -4944,14 +4944,14 @@
       <c r="U44" s="48"/>
     </row>
     <row r="45" spans="2:23" s="55" customFormat="1" ht="35.1" customHeight="1">
-      <c r="B45" s="318" t="s">
+      <c r="B45" s="380" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="273" t="s">
+      <c r="C45" s="382" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="274"/>
-      <c r="E45" s="275"/>
+      <c r="D45" s="383"/>
+      <c r="E45" s="384"/>
       <c r="F45" s="117"/>
       <c r="G45" s="132">
         <v>30</v>
@@ -4974,7 +4974,7 @@
       <c r="U45" s="48"/>
     </row>
     <row r="46" spans="2:23" s="55" customFormat="1" ht="35.1" customHeight="1">
-      <c r="B46" s="319"/>
+      <c r="B46" s="381"/>
       <c r="C46" s="237" t="s">
         <v>97</v>
       </c>
@@ -5062,14 +5062,14 @@
       <c r="U48" s="48"/>
     </row>
     <row r="49" spans="2:25" ht="35.1" customHeight="1">
-      <c r="B49" s="318" t="s">
+      <c r="B49" s="380" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="273" t="s">
+      <c r="C49" s="382" t="s">
         <v>114</v>
       </c>
-      <c r="D49" s="274"/>
-      <c r="E49" s="275"/>
+      <c r="D49" s="383"/>
+      <c r="E49" s="384"/>
       <c r="F49" s="44"/>
       <c r="G49" s="132">
         <v>34</v>
@@ -5092,7 +5092,7 @@
       <c r="U49" s="48"/>
     </row>
     <row r="50" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B50" s="319"/>
+      <c r="B50" s="381"/>
       <c r="C50" s="237" t="s">
         <v>97</v>
       </c>
@@ -5150,10 +5150,10 @@
       <c r="S51" s="45"/>
       <c r="T51" s="47"/>
       <c r="U51" s="48"/>
-      <c r="X51" s="321" t="s">
+      <c r="X51" s="345" t="s">
         <v>26</v>
       </c>
-      <c r="Y51" s="322"/>
+      <c r="Y51" s="346"/>
     </row>
     <row r="52" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
       <c r="B52" s="177" t="s">
@@ -5218,12 +5218,12 @@
       <c r="Y53" s="52"/>
     </row>
     <row r="54" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B54" s="287" t="s">
+      <c r="B54" s="347" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="288"/>
-      <c r="D54" s="291"/>
-      <c r="E54" s="292"/>
+      <c r="C54" s="393"/>
+      <c r="D54" s="395"/>
+      <c r="E54" s="396"/>
       <c r="F54" s="240"/>
       <c r="G54" s="132">
         <v>39</v>
@@ -5250,12 +5250,12 @@
       <c r="Y54" s="32"/>
     </row>
     <row r="55" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B55" s="285" t="s">
+      <c r="B55" s="391" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="286"/>
-      <c r="D55" s="293"/>
-      <c r="E55" s="294"/>
+      <c r="C55" s="392"/>
+      <c r="D55" s="397"/>
+      <c r="E55" s="398"/>
       <c r="F55" s="240"/>
       <c r="G55" s="133">
         <v>40</v>
@@ -5278,12 +5278,12 @@
       <c r="U55" s="62"/>
     </row>
     <row r="56" spans="2:25" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B56" s="289" t="s">
+      <c r="B56" s="349" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="290"/>
-      <c r="D56" s="282"/>
-      <c r="E56" s="283"/>
+      <c r="C56" s="394"/>
+      <c r="D56" s="308"/>
+      <c r="E56" s="389"/>
       <c r="F56" s="240"/>
       <c r="G56" s="238" t="s">
         <v>87</v>
@@ -5347,61 +5347,61 @@
       <c r="B58" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="C58" s="295"/>
-      <c r="D58" s="295"/>
-      <c r="E58" s="296"/>
-      <c r="F58" s="284"/>
-      <c r="G58" s="410" t="s">
+      <c r="C58" s="399"/>
+      <c r="D58" s="399"/>
+      <c r="E58" s="400"/>
+      <c r="F58" s="390"/>
+      <c r="G58" s="264" t="s">
         <v>136</v>
       </c>
-      <c r="H58" s="411"/>
-      <c r="I58" s="411"/>
-      <c r="J58" s="412"/>
-      <c r="K58" s="410" t="s">
+      <c r="H58" s="265"/>
+      <c r="I58" s="265"/>
+      <c r="J58" s="266"/>
+      <c r="K58" s="264" t="s">
         <v>146</v>
       </c>
-      <c r="L58" s="411"/>
-      <c r="M58" s="411"/>
-      <c r="N58" s="412"/>
+      <c r="L58" s="265"/>
+      <c r="M58" s="265"/>
+      <c r="N58" s="266"/>
       <c r="O58" s="253" t="s">
         <v>8</v>
       </c>
       <c r="P58" s="256" t="s">
         <v>155</v>
       </c>
-      <c r="Q58" s="406" t="s">
+      <c r="Q58" s="260" t="s">
         <v>148</v>
       </c>
-      <c r="R58" s="407"/>
-      <c r="S58" s="262" t="s">
+      <c r="R58" s="261"/>
+      <c r="S58" s="405" t="s">
         <v>152</v>
       </c>
-      <c r="T58" s="263"/>
-      <c r="U58" s="264"/>
+      <c r="T58" s="406"/>
+      <c r="U58" s="407"/>
     </row>
     <row r="59" spans="2:25" ht="28.5" customHeight="1">
       <c r="B59" s="25"/>
       <c r="C59" s="44"/>
       <c r="D59" s="44"/>
       <c r="E59" s="33"/>
-      <c r="F59" s="284"/>
+      <c r="F59" s="390"/>
       <c r="G59" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="H59" s="349" t="s">
+      <c r="H59" s="258" t="s">
         <v>138</v>
       </c>
-      <c r="I59" s="350"/>
+      <c r="I59" s="259"/>
       <c r="J59" s="182" t="s">
         <v>137</v>
       </c>
       <c r="K59" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="L59" s="349" t="s">
+      <c r="L59" s="258" t="s">
         <v>138</v>
       </c>
-      <c r="M59" s="350"/>
+      <c r="M59" s="259"/>
       <c r="N59" s="239" t="s">
         <v>137</v>
       </c>
@@ -5409,11 +5409,11 @@
         <v>1</v>
       </c>
       <c r="P59" s="255"/>
-      <c r="Q59" s="408"/>
-      <c r="R59" s="409"/>
-      <c r="S59" s="265"/>
-      <c r="T59" s="266"/>
-      <c r="U59" s="267"/>
+      <c r="Q59" s="262"/>
+      <c r="R59" s="263"/>
+      <c r="S59" s="408"/>
+      <c r="T59" s="344"/>
+      <c r="U59" s="409"/>
     </row>
     <row r="60" spans="2:25" ht="28.5" customHeight="1">
       <c r="B60" s="25"/>
@@ -5424,24 +5424,24 @@
       <c r="G60" s="183">
         <v>1</v>
       </c>
-      <c r="H60" s="271"/>
-      <c r="I60" s="272"/>
+      <c r="H60" s="329"/>
+      <c r="I60" s="330"/>
       <c r="J60" s="184"/>
       <c r="K60" s="183">
         <v>1</v>
       </c>
-      <c r="L60" s="271"/>
-      <c r="M60" s="272"/>
+      <c r="L60" s="329"/>
+      <c r="M60" s="330"/>
       <c r="N60" s="221"/>
       <c r="O60" s="65">
         <v>2</v>
       </c>
       <c r="P60" s="222"/>
-      <c r="Q60" s="258"/>
-      <c r="R60" s="259"/>
-      <c r="S60" s="265"/>
-      <c r="T60" s="266"/>
-      <c r="U60" s="267"/>
+      <c r="Q60" s="401"/>
+      <c r="R60" s="402"/>
+      <c r="S60" s="408"/>
+      <c r="T60" s="344"/>
+      <c r="U60" s="409"/>
     </row>
     <row r="61" spans="2:25" ht="28.5" customHeight="1">
       <c r="B61" s="25"/>
@@ -5452,24 +5452,24 @@
       <c r="G61" s="183">
         <v>2</v>
       </c>
-      <c r="H61" s="271"/>
-      <c r="I61" s="272"/>
+      <c r="H61" s="329"/>
+      <c r="I61" s="330"/>
       <c r="J61" s="184"/>
       <c r="K61" s="183">
         <v>2</v>
       </c>
-      <c r="L61" s="271"/>
-      <c r="M61" s="272"/>
+      <c r="L61" s="329"/>
+      <c r="M61" s="330"/>
       <c r="N61" s="221"/>
       <c r="O61" s="65">
         <v>3</v>
       </c>
       <c r="P61" s="222"/>
-      <c r="Q61" s="258"/>
-      <c r="R61" s="259"/>
-      <c r="S61" s="265"/>
-      <c r="T61" s="266"/>
-      <c r="U61" s="267"/>
+      <c r="Q61" s="401"/>
+      <c r="R61" s="402"/>
+      <c r="S61" s="408"/>
+      <c r="T61" s="344"/>
+      <c r="U61" s="409"/>
     </row>
     <row r="62" spans="2:25" ht="28.5" customHeight="1">
       <c r="B62" s="25"/>
@@ -5480,24 +5480,24 @@
       <c r="G62" s="183">
         <v>3</v>
       </c>
-      <c r="H62" s="271"/>
-      <c r="I62" s="272"/>
+      <c r="H62" s="329"/>
+      <c r="I62" s="330"/>
       <c r="J62" s="184"/>
       <c r="K62" s="183">
         <v>3</v>
       </c>
-      <c r="L62" s="271"/>
-      <c r="M62" s="272"/>
+      <c r="L62" s="329"/>
+      <c r="M62" s="330"/>
       <c r="N62" s="221"/>
       <c r="O62" s="65">
         <v>4</v>
       </c>
       <c r="P62" s="222"/>
-      <c r="Q62" s="258"/>
-      <c r="R62" s="259"/>
-      <c r="S62" s="265"/>
-      <c r="T62" s="266"/>
-      <c r="U62" s="267"/>
+      <c r="Q62" s="401"/>
+      <c r="R62" s="402"/>
+      <c r="S62" s="408"/>
+      <c r="T62" s="344"/>
+      <c r="U62" s="409"/>
     </row>
     <row r="63" spans="2:25" ht="28.5" customHeight="1">
       <c r="B63" s="25"/>
@@ -5508,24 +5508,24 @@
       <c r="G63" s="183">
         <v>4</v>
       </c>
-      <c r="H63" s="271"/>
-      <c r="I63" s="272"/>
+      <c r="H63" s="329"/>
+      <c r="I63" s="330"/>
       <c r="J63" s="184"/>
       <c r="K63" s="183">
         <v>4</v>
       </c>
-      <c r="L63" s="271"/>
-      <c r="M63" s="272"/>
+      <c r="L63" s="329"/>
+      <c r="M63" s="330"/>
       <c r="N63" s="221"/>
       <c r="O63" s="65">
         <v>5</v>
       </c>
       <c r="P63" s="222"/>
-      <c r="Q63" s="258"/>
-      <c r="R63" s="259"/>
-      <c r="S63" s="265"/>
-      <c r="T63" s="266"/>
-      <c r="U63" s="267"/>
+      <c r="Q63" s="401"/>
+      <c r="R63" s="402"/>
+      <c r="S63" s="408"/>
+      <c r="T63" s="344"/>
+      <c r="U63" s="409"/>
     </row>
     <row r="64" spans="2:25" ht="28.5" customHeight="1">
       <c r="B64" s="25"/>
@@ -5536,24 +5536,24 @@
       <c r="G64" s="183">
         <v>5</v>
       </c>
-      <c r="H64" s="271"/>
-      <c r="I64" s="272"/>
+      <c r="H64" s="329"/>
+      <c r="I64" s="330"/>
       <c r="J64" s="184"/>
       <c r="K64" s="183">
         <v>5</v>
       </c>
-      <c r="L64" s="271"/>
-      <c r="M64" s="272"/>
+      <c r="L64" s="329"/>
+      <c r="M64" s="330"/>
       <c r="N64" s="221"/>
       <c r="O64" s="65">
         <v>6</v>
       </c>
       <c r="P64" s="222"/>
-      <c r="Q64" s="258"/>
-      <c r="R64" s="259"/>
-      <c r="S64" s="265"/>
-      <c r="T64" s="266"/>
-      <c r="U64" s="267"/>
+      <c r="Q64" s="401"/>
+      <c r="R64" s="402"/>
+      <c r="S64" s="408"/>
+      <c r="T64" s="344"/>
+      <c r="U64" s="409"/>
     </row>
     <row r="65" spans="2:35" ht="28.5" customHeight="1">
       <c r="B65" s="25"/>
@@ -5564,24 +5564,24 @@
       <c r="G65" s="183">
         <v>6</v>
       </c>
-      <c r="H65" s="271"/>
-      <c r="I65" s="272"/>
+      <c r="H65" s="329"/>
+      <c r="I65" s="330"/>
       <c r="J65" s="184"/>
       <c r="K65" s="183">
         <v>6</v>
       </c>
-      <c r="L65" s="271"/>
-      <c r="M65" s="272"/>
+      <c r="L65" s="329"/>
+      <c r="M65" s="330"/>
       <c r="N65" s="221"/>
       <c r="O65" s="65">
         <v>7</v>
       </c>
       <c r="P65" s="222"/>
-      <c r="Q65" s="258"/>
-      <c r="R65" s="259"/>
-      <c r="S65" s="265"/>
-      <c r="T65" s="266"/>
-      <c r="U65" s="267"/>
+      <c r="Q65" s="401"/>
+      <c r="R65" s="402"/>
+      <c r="S65" s="408"/>
+      <c r="T65" s="344"/>
+      <c r="U65" s="409"/>
     </row>
     <row r="66" spans="2:35" ht="28.5" customHeight="1" thickBot="1">
       <c r="B66" s="207"/>
@@ -5592,24 +5592,24 @@
       <c r="G66" s="236">
         <v>7</v>
       </c>
-      <c r="H66" s="282"/>
-      <c r="I66" s="297"/>
+      <c r="H66" s="308"/>
+      <c r="I66" s="309"/>
       <c r="J66" s="242"/>
       <c r="K66" s="236">
         <v>7</v>
       </c>
-      <c r="L66" s="282"/>
-      <c r="M66" s="297"/>
+      <c r="L66" s="308"/>
+      <c r="M66" s="309"/>
       <c r="N66" s="150"/>
       <c r="O66" s="66">
         <v>8</v>
       </c>
       <c r="P66" s="223"/>
-      <c r="Q66" s="260"/>
-      <c r="R66" s="261"/>
-      <c r="S66" s="268"/>
-      <c r="T66" s="269"/>
-      <c r="U66" s="270"/>
+      <c r="Q66" s="403"/>
+      <c r="R66" s="404"/>
+      <c r="S66" s="410"/>
+      <c r="T66" s="411"/>
+      <c r="U66" s="412"/>
     </row>
     <row r="67" spans="2:35" ht="21.95" customHeight="1">
       <c r="B67" s="219"/>
@@ -7687,26 +7687,65 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="Q59:R59"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="B1:U1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:U14"/>
-    <mergeCell ref="S8:U10"/>
-    <mergeCell ref="S12:U13"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="Q65:R65"/>
+    <mergeCell ref="Q66:R66"/>
+    <mergeCell ref="S58:U66"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="Z21:AA22"/>
+    <mergeCell ref="X51:Y51"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="X19:AA19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R11:R13"/>
     <mergeCell ref="L66:M66"/>
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="Q7:R7"/>
@@ -7723,65 +7762,26 @@
     <mergeCell ref="L60:M60"/>
     <mergeCell ref="L61:M61"/>
     <mergeCell ref="L62:M62"/>
-    <mergeCell ref="L63:M63"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="Z21:AA22"/>
-    <mergeCell ref="X51:Y51"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="X19:AA19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="Q66:R66"/>
-    <mergeCell ref="S58:U66"/>
-    <mergeCell ref="Q60:R60"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:U14"/>
+    <mergeCell ref="S8:U10"/>
+    <mergeCell ref="S12:U13"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="Q59:R59"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="K58:N58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0" top="0" bottom="7.874015748031496E-2" header="0" footer="0"/>
@@ -7801,10 +7801,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:J48"/>
+  <dimension ref="B1:K48"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -7820,7 +7820,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
+    <row r="1" spans="2:11">
       <c r="F1" s="245"/>
       <c r="G1" s="248">
         <v>12.34</v>
@@ -7829,7 +7829,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:11">
       <c r="F2" s="245"/>
       <c r="G2" s="248">
         <v>7.28</v>
@@ -7839,21 +7839,21 @@
       </c>
       <c r="J2" s="250"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:11">
       <c r="F3" s="245"/>
       <c r="G3" s="248"/>
       <c r="H3" s="247">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="18" customHeight="1" thickBot="1">
+    <row r="4" spans="2:11" ht="18" customHeight="1" thickBot="1">
       <c r="F4" s="245"/>
       <c r="G4" s="248"/>
       <c r="H4" s="247">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="17.25" customHeight="1">
+    <row r="5" spans="2:11" ht="17.25" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="20.25" customHeight="1">
+    <row r="6" spans="2:11" ht="20.25" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="20.25" customHeight="1">
+    <row r="7" spans="2:11" ht="20.25" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="20.25" customHeight="1">
+    <row r="8" spans="2:11" ht="20.25" customHeight="1">
       <c r="B8" s="8" t="s">
         <v>39</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="20.25" customHeight="1">
+    <row r="9" spans="2:11" ht="20.25" customHeight="1">
       <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="20.25" customHeight="1">
+    <row r="10" spans="2:11" ht="20.25" customHeight="1">
       <c r="B10" s="8" t="s">
         <v>41</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="20.25" customHeight="1">
+    <row r="11" spans="2:11" ht="20.25" customHeight="1">
       <c r="B11" s="8" t="s">
         <v>43</v>
       </c>
@@ -7957,8 +7957,12 @@
         <f>IFERROR(D20*D10/D24,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="2:10" ht="20.25" customHeight="1">
+      <c r="K11" s="1">
+        <f>D11*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="20.25" customHeight="1">
       <c r="B12" s="8" t="s">
         <v>44</v>
       </c>
@@ -7981,7 +7985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="20.25" customHeight="1">
+    <row r="13" spans="2:11" ht="20.25" customHeight="1">
       <c r="B13" s="8" t="s">
         <v>46</v>
       </c>
@@ -8002,7 +8006,7 @@
         <v>°-℃/m</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="20.25" customHeight="1">
+    <row r="14" spans="2:11" ht="20.25" customHeight="1">
       <c r="B14" s="8" t="s">
         <v>48</v>
       </c>
@@ -8021,7 +8025,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="20.25" customHeight="1">
+    <row r="15" spans="2:11" ht="20.25" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>49</v>
       </c>
@@ -8034,7 +8038,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="25.5" customHeight="1">
+    <row r="16" spans="2:11" ht="25.5" customHeight="1">
       <c r="B16" s="8" t="s">
         <v>50</v>
       </c>

</xml_diff>